<commit_message>
Pictures & new contacts added for demo
</commit_message>
<xml_diff>
--- a/ProjectSmartphone_BriceBerclazSamuelMichellod/HoursSpentOnTheProject.xlsx
+++ b/ProjectSmartphone_BriceBerclazSamuelMichellod/HoursSpentOnTheProject.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brice\git\BerclazMichellodSmartphone\ProjectSmartphone\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brice\git\BerclazMichellodSmartphone\ProjectSmartphone_BriceBerclazSamuelMichellod\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97F3D3B7-F7EA-4E96-8389-C38B9F48417F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C297BD3-5A7B-4872-BFE9-43646ABA960F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{71573441-F5A1-4DC6-AB90-1F7E44CCBFE6}"/>
   </bookViews>
@@ -76,7 +76,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,13 +104,6 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -373,13 +366,7 @@
   </cellStyleXfs>
   <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -428,6 +415,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -457,27 +450,6 @@
         </right>
         <vertical/>
       </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color theme="1"/>
-        <name val="Consolas"/>
-        <family val="3"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -509,6 +481,41 @@
     </dxf>
     <dxf>
       <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
         <b/>
         <i val="0"/>
         <strike val="0"/>
@@ -519,20 +526,6 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color theme="1"/>
-        <name val="Consolas"/>
-        <family val="3"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
         <color theme="1"/>
         <name val="Consolas"/>
         <family val="3"/>
@@ -554,11 +547,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A7785400-1D6C-4B88-8D1C-22437BE1B7A7}" name="Tableau1" displayName="Tableau1" ref="A2:D11" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4" headerRowBorderDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A7785400-1D6C-4B88-8D1C-22437BE1B7A7}" name="Tableau1" displayName="Tableau1" ref="A2:D11" totalsRowShown="0" headerRowDxfId="6" dataDxfId="4" headerRowBorderDxfId="5">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{060F5554-9A93-462C-B5ED-41F717A94850}" name="Apps" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{F13EC6CA-1FC0-4EF4-8BE0-30817AB31B0F}" name="TIME - Brice" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{C38037F2-0F9F-4C3A-9CA4-3BA8524BEE48}" name="TIME - Samuel" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{060F5554-9A93-462C-B5ED-41F717A94850}" name="Apps" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{F13EC6CA-1FC0-4EF4-8BE0-30817AB31B0F}" name="TIME - Brice" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{C38037F2-0F9F-4C3A-9CA4-3BA8524BEE48}" name="TIME - Samuel" dataDxfId="1"/>
     <tableColumn id="4" xr3:uid="{C1A9B5D4-9F35-47CC-AD8D-A95FA77AB1CA}" name="TOTAL TIME" dataDxfId="0">
       <calculatedColumnFormula>SUM(B3:C3)</calculatedColumnFormula>
     </tableColumn>
@@ -867,7 +860,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -879,162 +872,162 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="7">
         <v>8</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="8">
         <v>0</v>
       </c>
-      <c r="D3" s="11">
+      <c r="D3" s="9">
         <f>SUM(B3:C3)</f>
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="13">
-        <v>15</v>
-      </c>
-      <c r="C4" s="14">
+      <c r="B4" s="11">
+        <v>14</v>
+      </c>
+      <c r="C4" s="12">
         <v>0</v>
       </c>
-      <c r="D4" s="15">
+      <c r="D4" s="13">
         <f t="shared" ref="D4:D11" si="0">SUM(B4:C4)</f>
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="13">
-        <v>10</v>
-      </c>
-      <c r="C5" s="14">
+      <c r="B5" s="11">
+        <v>15</v>
+      </c>
+      <c r="C5" s="12">
         <v>0</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="13">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="13">
+      <c r="B6" s="11">
         <v>0</v>
       </c>
-      <c r="C6" s="14">
-        <v>10</v>
-      </c>
-      <c r="D6" s="15">
+      <c r="C6" s="12">
+        <v>14</v>
+      </c>
+      <c r="D6" s="13">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="13">
+      <c r="B7" s="11">
         <v>0</v>
       </c>
-      <c r="C7" s="14">
+      <c r="C7" s="12">
         <v>2</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="13">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="13">
+      <c r="B8" s="11">
         <v>3</v>
       </c>
-      <c r="C8" s="14">
+      <c r="C8" s="12">
         <v>15</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D8" s="13">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="13">
-        <v>20</v>
-      </c>
-      <c r="C9" s="14">
+      <c r="B9" s="11">
+        <v>24</v>
+      </c>
+      <c r="C9" s="12">
         <v>0</v>
       </c>
-      <c r="D9" s="15">
+      <c r="D9" s="13">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="17">
-        <v>10</v>
-      </c>
-      <c r="C10" s="18">
+      <c r="B10" s="15">
+        <v>12</v>
+      </c>
+      <c r="C10" s="16">
         <v>15</v>
       </c>
-      <c r="D10" s="19">
+      <c r="D10" s="17">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="4" t="s">
+    <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="4">
         <f>SUM(B3:B10)</f>
-        <v>66</v>
-      </c>
-      <c r="C11" s="6">
+        <v>76</v>
+      </c>
+      <c r="C11" s="4">
         <f>SUM(C3:C10)</f>
-        <v>42</v>
-      </c>
-      <c r="D11" s="3">
+        <v>46</v>
+      </c>
+      <c r="D11" s="19">
         <f t="shared" si="0"/>
-        <v>108</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>